<commit_message>
create account test done
create account test done
</commit_message>
<xml_diff>
--- a/CRMTelecomProject/src/main/java/com/TestData/CRM Credential.xlsx
+++ b/CRMTelecomProject/src/main/java/com/TestData/CRM Credential.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0F6F94C8-4E43-44C1-AC88-DDA7B4599012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A392306A-35CB-4DF2-887D-0093272D8ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9A16DF2D-FCEE-47EC-8348-93CFED6DFD64}"/>
   </bookViews>
@@ -16,20 +16,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>username</t>
   </si>
@@ -389,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6119469-AC4B-4FF3-9541-E1986F87FC9F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,6 +409,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>